<commit_message>
added benchmarks for Google Play results
</commit_message>
<xml_diff>
--- a/UBCBench Results.xlsx
+++ b/UBCBench Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\eDocs\MASc\ISSTA\UBCBench\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\eDocs\MASc\ISSTA\UBCBenchNew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8226B066-ACE3-4ED9-97DC-B66C65A199EA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A249D5B5-C931-4ED6-9BE8-9EB97107B88B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6225" yWindow="17250" windowWidth="24375" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
   <si>
     <t>UBCBench</t>
   </si>
@@ -147,9 +147,6 @@
     <t>ViewCasting</t>
   </si>
   <si>
-    <t>ConservativeModel</t>
-  </si>
-  <si>
     <t>GetClass</t>
   </si>
   <si>
@@ -159,7 +156,31 @@
     <t>SendTextMessage</t>
   </si>
   <si>
-    <t>CastingForward</t>
+    <t>ConservativeModel1</t>
+  </si>
+  <si>
+    <t>ConservativeModel2</t>
+  </si>
+  <si>
+    <t>ConservativeModel3</t>
+  </si>
+  <si>
+    <t>SetContentView</t>
+  </si>
+  <si>
+    <t>CallbacksInFragment</t>
+  </si>
+  <si>
+    <t>GetConstructor</t>
+  </si>
+  <si>
+    <t>ContextSensitivityDepth</t>
+  </si>
+  <si>
+    <t>DuplicatedFlows</t>
+  </si>
+  <si>
+    <t>DroidSafe is flow insensitive, leading to two FPs</t>
   </si>
 </sst>
 </file>
@@ -175,18 +196,15 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -589,11 +607,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:W1011"/>
+  <dimension ref="A1:W1017"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U24" sqref="U24"/>
+      <pane xSplit="5" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -873,7 +891,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -1066,7 +1084,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -1126,513 +1144,519 @@
       </c>
       <c r="W9" s="8"/>
     </row>
-    <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="16"/>
-      <c r="R10" s="16"/>
-      <c r="S10" s="16"/>
-      <c r="T10" s="16"/>
-      <c r="U10" s="16"/>
-      <c r="V10" s="16"/>
-      <c r="W10" s="16"/>
+    <row r="10" spans="1:23" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
+        <v>7</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1</v>
+      </c>
+      <c r="G10" s="6">
+        <v>1</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0</v>
+      </c>
+      <c r="I10" s="6">
+        <v>1</v>
+      </c>
+      <c r="J10" s="8">
+        <v>0</v>
+      </c>
+      <c r="K10" s="8"/>
+      <c r="L10" s="6">
+        <v>1</v>
+      </c>
+      <c r="M10" s="6">
+        <v>1</v>
+      </c>
+      <c r="N10" s="6">
+        <v>1</v>
+      </c>
+      <c r="O10" s="6">
+        <v>0</v>
+      </c>
+      <c r="P10" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="6">
+        <v>1</v>
+      </c>
+      <c r="S10" s="6">
+        <v>1</v>
+      </c>
+      <c r="T10" s="6">
+        <v>1</v>
+      </c>
+      <c r="U10" s="6">
+        <v>0</v>
+      </c>
+      <c r="V10" s="6">
+        <v>0</v>
+      </c>
+      <c r="W10" s="8"/>
     </row>
     <row r="11" spans="1:23" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
-        <v>1</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="5">
-        <v>1</v>
-      </c>
-      <c r="D11" s="5">
-        <v>1</v>
-      </c>
-      <c r="E11" s="5">
-        <v>1</v>
-      </c>
-      <c r="F11" s="5">
-        <v>1</v>
-      </c>
-      <c r="G11" s="5">
-        <v>1</v>
-      </c>
-      <c r="H11" s="5">
-        <v>1</v>
-      </c>
-      <c r="I11" s="5">
-        <v>0</v>
-      </c>
-      <c r="J11" s="5">
-        <v>0</v>
-      </c>
-      <c r="K11" s="11"/>
-      <c r="L11" s="5">
-        <v>1</v>
-      </c>
-      <c r="M11" s="5">
-        <v>1</v>
-      </c>
-      <c r="N11" s="5">
-        <v>1</v>
-      </c>
-      <c r="O11" s="5">
-        <v>0</v>
-      </c>
-      <c r="P11" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="5">
-        <v>1</v>
-      </c>
-      <c r="S11" s="5">
-        <v>1</v>
-      </c>
-      <c r="T11" s="5">
-        <v>1</v>
-      </c>
-      <c r="U11" s="5">
-        <v>0</v>
-      </c>
-      <c r="V11" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+        <v>8</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1</v>
+      </c>
+      <c r="H11" s="6">
+        <v>1</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0</v>
+      </c>
+      <c r="J11" s="8">
+        <v>1</v>
+      </c>
+      <c r="K11" s="8"/>
+      <c r="L11" s="6">
+        <v>1</v>
+      </c>
+      <c r="M11" s="6">
+        <v>1</v>
+      </c>
+      <c r="N11" s="6">
+        <v>0</v>
+      </c>
+      <c r="O11" s="6">
+        <v>0</v>
+      </c>
+      <c r="P11" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="6">
+        <v>1</v>
+      </c>
+      <c r="S11" s="6">
+        <v>1</v>
+      </c>
+      <c r="T11" s="6">
+        <v>0</v>
+      </c>
+      <c r="U11" s="6">
+        <v>0</v>
+      </c>
+      <c r="V11" s="6">
+        <v>0</v>
+      </c>
+      <c r="W11" s="8"/>
+    </row>
+    <row r="12" spans="1:23" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
+        <v>9</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="6">
+        <v>1</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0</v>
+      </c>
+      <c r="I12" s="6">
+        <v>1</v>
+      </c>
+      <c r="J12" s="8">
+        <v>0</v>
+      </c>
+      <c r="K12" s="8"/>
+      <c r="L12" s="6">
+        <v>0</v>
+      </c>
+      <c r="M12" s="6">
+        <v>0</v>
+      </c>
+      <c r="N12" s="6">
+        <v>0</v>
+      </c>
+      <c r="O12" s="6">
+        <v>1</v>
+      </c>
+      <c r="P12" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="6">
+        <v>0</v>
+      </c>
+      <c r="S12" s="6">
+        <v>0</v>
+      </c>
+      <c r="T12" s="6">
+        <v>0</v>
+      </c>
+      <c r="U12" s="6">
+        <v>1</v>
+      </c>
+      <c r="V12" s="6">
+        <v>0</v>
+      </c>
+      <c r="W12" s="8"/>
+    </row>
+    <row r="13" spans="1:23" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>10</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="6">
         <v>2</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="D13" s="6">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3">
+        <v>2</v>
+      </c>
+      <c r="F13" s="6">
+        <v>1</v>
+      </c>
+      <c r="G13" s="6">
+        <v>2</v>
+      </c>
+      <c r="H13" s="6">
+        <v>1</v>
+      </c>
+      <c r="I13" s="6">
+        <v>1</v>
+      </c>
+      <c r="J13" s="8">
+        <v>0</v>
+      </c>
+      <c r="K13" s="8"/>
+      <c r="L13" s="6">
+        <v>1</v>
+      </c>
+      <c r="M13" s="6">
+        <v>2</v>
+      </c>
+      <c r="N13" s="6">
+        <v>1</v>
+      </c>
+      <c r="O13" s="6">
+        <v>1</v>
+      </c>
+      <c r="P13" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="6">
+        <v>2</v>
+      </c>
+      <c r="S13" s="6">
+        <v>2</v>
+      </c>
+      <c r="T13" s="6">
+        <v>4</v>
+      </c>
+      <c r="U13" s="6">
+        <v>0</v>
+      </c>
+      <c r="V13" s="6">
+        <v>2</v>
+      </c>
+      <c r="W13" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>11</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0</v>
+      </c>
+      <c r="H14" s="6">
+        <v>0</v>
+      </c>
+      <c r="I14" s="6">
+        <v>1</v>
+      </c>
+      <c r="J14" s="8">
+        <v>0</v>
+      </c>
+      <c r="K14" s="8"/>
+      <c r="L14" s="6">
+        <v>0</v>
+      </c>
+      <c r="M14" s="6">
+        <v>0</v>
+      </c>
+      <c r="N14" s="6">
+        <v>0</v>
+      </c>
+      <c r="O14" s="6">
+        <v>1</v>
+      </c>
+      <c r="P14" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="6">
+        <v>0</v>
+      </c>
+      <c r="S14" s="6">
+        <v>0</v>
+      </c>
+      <c r="T14" s="6">
+        <v>0</v>
+      </c>
+      <c r="U14" s="6">
+        <v>1</v>
+      </c>
+      <c r="V14" s="6">
+        <v>0</v>
+      </c>
+      <c r="W14" s="8"/>
+    </row>
+    <row r="15" spans="1:23" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
+        <v>12</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="6">
+        <v>1</v>
+      </c>
+      <c r="D15" s="6">
+        <v>3</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1</v>
+      </c>
+      <c r="G15" s="6">
+        <v>3</v>
+      </c>
+      <c r="H15" s="6">
+        <v>1</v>
+      </c>
+      <c r="I15" s="6">
+        <v>0</v>
+      </c>
+      <c r="J15" s="8">
+        <v>0</v>
+      </c>
+      <c r="K15" s="8"/>
+      <c r="L15" s="6">
+        <v>1</v>
+      </c>
+      <c r="M15" s="6">
+        <v>3</v>
+      </c>
+      <c r="N15" s="6">
+        <v>2</v>
+      </c>
+      <c r="O15" s="6">
+        <v>0</v>
+      </c>
+      <c r="P15" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="6">
+        <v>1</v>
+      </c>
+      <c r="S15" s="6">
+        <v>3</v>
+      </c>
+      <c r="T15" s="6">
+        <v>3</v>
+      </c>
+      <c r="U15" s="6">
+        <v>0</v>
+      </c>
+      <c r="V15" s="6">
+        <v>3</v>
+      </c>
+      <c r="W15" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
+        <v>13</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="6">
+        <v>1</v>
+      </c>
+      <c r="D16" s="6">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
+      <c r="F16" s="6">
+        <v>1</v>
+      </c>
+      <c r="G16" s="6">
+        <v>1</v>
+      </c>
+      <c r="H16" s="6">
+        <v>1</v>
+      </c>
+      <c r="I16" s="6">
+        <v>0</v>
+      </c>
+      <c r="J16" s="8">
+        <v>0</v>
+      </c>
+      <c r="K16" s="8"/>
+      <c r="L16" s="6">
+        <v>1</v>
+      </c>
+      <c r="M16" s="6">
+        <v>1</v>
+      </c>
+      <c r="N16" s="6">
+        <v>2</v>
+      </c>
+      <c r="O16" s="6">
+        <v>0</v>
+      </c>
+      <c r="P16" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="6">
+        <v>1</v>
+      </c>
+      <c r="S16" s="6">
+        <v>1</v>
+      </c>
+      <c r="T16" s="6">
+        <v>1</v>
+      </c>
+      <c r="U16" s="6">
+        <v>0</v>
+      </c>
+      <c r="V16" s="6">
+        <v>0</v>
+      </c>
+      <c r="W16" s="8"/>
+    </row>
+    <row r="17" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="16"/>
+      <c r="V17" s="16"/>
+      <c r="W17" s="16"/>
+    </row>
+    <row r="18" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>1</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="5">
-        <v>1</v>
-      </c>
-      <c r="D12" s="5">
+      <c r="C18" s="5">
+        <v>1</v>
+      </c>
+      <c r="D18" s="5">
         <v>2</v>
       </c>
-      <c r="E12" s="5">
-        <v>1</v>
-      </c>
-      <c r="F12" s="5">
-        <v>1</v>
-      </c>
-      <c r="G12" s="5">
+      <c r="E18" s="5">
+        <v>1</v>
+      </c>
+      <c r="F18" s="5">
+        <v>1</v>
+      </c>
+      <c r="G18" s="5">
         <v>2</v>
       </c>
-      <c r="H12" s="5">
-        <v>1</v>
-      </c>
-      <c r="I12" s="5">
-        <v>0</v>
-      </c>
-      <c r="J12" s="5">
-        <v>0</v>
-      </c>
-      <c r="K12" s="11"/>
-      <c r="L12" s="5">
-        <v>1</v>
-      </c>
-      <c r="M12" s="5">
-        <v>5</v>
-      </c>
-      <c r="N12" s="5">
-        <v>1</v>
-      </c>
-      <c r="O12" s="5">
-        <v>0</v>
-      </c>
-      <c r="P12" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="5">
-        <v>1</v>
-      </c>
-      <c r="S12" s="5">
-        <v>2</v>
-      </c>
-      <c r="T12" s="5">
-        <v>1</v>
-      </c>
-      <c r="U12" s="5">
-        <v>0</v>
-      </c>
-      <c r="V12" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
-        <v>3</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="2">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2">
-        <v>1</v>
-      </c>
-      <c r="E13" s="3">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2">
-        <v>1</v>
-      </c>
-      <c r="G13" s="2">
-        <v>1</v>
-      </c>
-      <c r="H13" s="2">
-        <v>1</v>
-      </c>
-      <c r="I13" s="2">
-        <v>0</v>
-      </c>
-      <c r="J13" s="8">
-        <v>0</v>
-      </c>
-      <c r="K13" s="10"/>
-      <c r="L13" s="2">
-        <v>0</v>
-      </c>
-      <c r="M13" s="2">
-        <v>1</v>
-      </c>
-      <c r="N13" s="2">
-        <v>0</v>
-      </c>
-      <c r="O13" s="2">
-        <v>1</v>
-      </c>
-      <c r="P13" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="2">
-        <v>1</v>
-      </c>
-      <c r="S13" s="2">
-        <v>1</v>
-      </c>
-      <c r="T13" s="2">
-        <v>1</v>
-      </c>
-      <c r="U13" s="2">
-        <v>0</v>
-      </c>
-      <c r="V13" s="2">
-        <v>0</v>
-      </c>
-      <c r="W13" s="8"/>
-    </row>
-    <row r="14" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
-        <v>4</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="5">
-        <v>1</v>
-      </c>
-      <c r="D14" s="5">
-        <v>1</v>
-      </c>
-      <c r="E14" s="5">
-        <v>0</v>
-      </c>
-      <c r="F14" s="5">
-        <v>0</v>
-      </c>
-      <c r="G14" s="5">
-        <v>1</v>
-      </c>
-      <c r="H14" s="5">
-        <v>0</v>
-      </c>
-      <c r="I14" s="5">
-        <v>0</v>
-      </c>
-      <c r="J14" s="5">
-        <v>0</v>
-      </c>
-      <c r="K14" s="11"/>
-      <c r="L14" s="5">
-        <v>1</v>
-      </c>
-      <c r="M14" s="5">
-        <v>2</v>
-      </c>
-      <c r="N14" s="5">
-        <v>1</v>
-      </c>
-      <c r="O14" s="5">
-        <v>0</v>
-      </c>
-      <c r="P14" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="R14" s="5">
-        <v>1</v>
-      </c>
-      <c r="S14" s="5">
-        <v>1</v>
-      </c>
-      <c r="T14" s="5">
-        <v>0</v>
-      </c>
-      <c r="U14" s="5">
-        <v>0</v>
-      </c>
-      <c r="V14" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
-        <v>5</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="2">
-        <v>1</v>
-      </c>
-      <c r="D15" s="2">
-        <v>2</v>
-      </c>
-      <c r="E15" s="3">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2">
-        <v>1</v>
-      </c>
-      <c r="G15" s="2">
-        <v>2</v>
-      </c>
-      <c r="H15" s="2">
-        <v>1</v>
-      </c>
-      <c r="I15" s="2">
-        <v>0</v>
-      </c>
-      <c r="J15" s="8">
-        <v>0</v>
-      </c>
-      <c r="K15" s="10"/>
-      <c r="L15" s="2">
-        <v>1</v>
-      </c>
-      <c r="M15" s="2">
-        <v>2</v>
-      </c>
-      <c r="N15" s="2">
-        <v>2</v>
-      </c>
-      <c r="O15" s="2">
-        <v>0</v>
-      </c>
-      <c r="P15" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="2">
-        <v>1</v>
-      </c>
-      <c r="S15" s="2">
-        <v>2</v>
-      </c>
-      <c r="T15" s="2">
-        <v>1</v>
-      </c>
-      <c r="U15" s="2">
-        <v>0</v>
-      </c>
-      <c r="V15" s="2">
-        <v>0</v>
-      </c>
-      <c r="W15" s="8"/>
-    </row>
-    <row r="16" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6">
-        <v>6</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="2">
-        <v>1</v>
-      </c>
-      <c r="D16" s="2">
-        <v>1</v>
-      </c>
-      <c r="E16" s="3">
-        <v>1</v>
-      </c>
-      <c r="F16" s="2">
-        <v>1</v>
-      </c>
-      <c r="G16" s="2">
-        <v>1</v>
-      </c>
-      <c r="H16" s="2">
-        <v>1</v>
-      </c>
-      <c r="I16" s="2">
-        <v>0</v>
-      </c>
-      <c r="J16" s="8">
-        <v>0</v>
-      </c>
-      <c r="K16" s="10"/>
-      <c r="L16" s="2">
-        <v>1</v>
-      </c>
-      <c r="M16" s="2">
-        <v>1</v>
-      </c>
-      <c r="N16" s="2">
-        <v>1</v>
-      </c>
-      <c r="O16" s="2">
-        <v>0</v>
-      </c>
-      <c r="P16" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="2">
-        <v>1</v>
-      </c>
-      <c r="S16" s="2">
-        <v>1</v>
-      </c>
-      <c r="T16" s="2">
-        <v>1</v>
-      </c>
-      <c r="U16" s="2">
-        <v>0</v>
-      </c>
-      <c r="V16" s="2">
-        <v>0</v>
-      </c>
-      <c r="W16" s="8"/>
-    </row>
-    <row r="17" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6">
-        <v>7</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="5">
-        <v>1</v>
-      </c>
-      <c r="D17" s="5">
-        <v>1</v>
-      </c>
-      <c r="E17" s="5">
-        <v>1</v>
-      </c>
-      <c r="F17" s="5">
-        <v>1</v>
-      </c>
-      <c r="G17" s="5">
-        <v>1</v>
-      </c>
-      <c r="H17" s="5">
-        <v>0</v>
-      </c>
-      <c r="I17" s="5">
-        <v>1</v>
-      </c>
-      <c r="J17" s="5">
-        <v>0</v>
-      </c>
-      <c r="K17" s="11"/>
-      <c r="L17" s="5">
-        <v>1</v>
-      </c>
-      <c r="M17" s="5">
-        <v>2</v>
-      </c>
-      <c r="N17" s="5">
-        <v>0</v>
-      </c>
-      <c r="O17" s="5">
-        <v>1</v>
-      </c>
-      <c r="P17" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="5">
-        <v>1</v>
-      </c>
-      <c r="S17" s="5">
-        <v>1</v>
-      </c>
-      <c r="T17" s="5">
-        <v>1</v>
-      </c>
-      <c r="U17" s="5">
-        <v>0</v>
-      </c>
-      <c r="V17" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6">
-        <v>8</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="5">
-        <v>1</v>
-      </c>
-      <c r="D18" s="5">
-        <v>1</v>
-      </c>
-      <c r="E18" s="5">
-        <v>1</v>
-      </c>
-      <c r="F18" s="5">
-        <v>1</v>
-      </c>
-      <c r="G18" s="5">
-        <v>1</v>
-      </c>
       <c r="H18" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" s="5">
         <v>0</v>
@@ -1642,13 +1666,13 @@
         <v>1</v>
       </c>
       <c r="M18" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N18" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O18" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P18" s="5">
         <v>0</v>
@@ -1658,7 +1682,7 @@
         <v>1</v>
       </c>
       <c r="S18" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T18" s="5">
         <v>1</v>
@@ -1671,239 +1695,278 @@
       </c>
     </row>
     <row r="19" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6">
-        <v>9</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="5">
-        <v>1</v>
-      </c>
-      <c r="D19" s="5">
-        <v>1</v>
-      </c>
-      <c r="E19" s="5">
-        <v>1</v>
-      </c>
-      <c r="F19" s="5">
-        <v>1</v>
-      </c>
-      <c r="G19" s="5">
-        <v>1</v>
-      </c>
-      <c r="H19" s="5">
-        <v>1</v>
-      </c>
-      <c r="I19" s="5">
-        <v>0</v>
-      </c>
-      <c r="J19" s="5">
-        <v>0</v>
-      </c>
-      <c r="K19" s="11"/>
-      <c r="L19" s="5">
-        <v>1</v>
-      </c>
-      <c r="M19" s="5">
+      <c r="A19" s="2">
         <v>2</v>
       </c>
-      <c r="N19" s="5">
-        <v>1</v>
-      </c>
-      <c r="O19" s="5">
-        <v>0</v>
-      </c>
-      <c r="P19" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="11"/>
-      <c r="R19" s="5">
-        <v>1</v>
-      </c>
-      <c r="S19" s="5">
-        <v>1</v>
-      </c>
-      <c r="T19" s="5">
-        <v>1</v>
-      </c>
-      <c r="U19" s="5">
-        <v>0</v>
-      </c>
-      <c r="V19" s="5">
-        <v>0</v>
-      </c>
+      <c r="B19" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2">
+        <v>1</v>
+      </c>
+      <c r="H19" s="2">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0</v>
+      </c>
+      <c r="J19" s="8">
+        <v>0</v>
+      </c>
+      <c r="K19" s="10"/>
+      <c r="L19" s="2">
+        <v>0</v>
+      </c>
+      <c r="M19" s="2">
+        <v>1</v>
+      </c>
+      <c r="N19" s="2">
+        <v>0</v>
+      </c>
+      <c r="O19" s="2">
+        <v>1</v>
+      </c>
+      <c r="P19" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="2">
+        <v>1</v>
+      </c>
+      <c r="S19" s="2">
+        <v>1</v>
+      </c>
+      <c r="T19" s="2">
+        <v>1</v>
+      </c>
+      <c r="U19" s="2">
+        <v>0</v>
+      </c>
+      <c r="V19" s="2">
+        <v>0</v>
+      </c>
+      <c r="W19" s="8"/>
     </row>
     <row r="20" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="15"/>
-      <c r="S20" s="15"/>
-      <c r="T20" s="15"/>
-      <c r="U20" s="15"/>
-      <c r="V20" s="15"/>
-      <c r="W20" s="15"/>
+      <c r="A20" s="2">
+        <v>3</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5">
+        <v>1</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0</v>
+      </c>
+      <c r="G20" s="5">
+        <v>1</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0</v>
+      </c>
+      <c r="I20" s="5">
+        <v>0</v>
+      </c>
+      <c r="J20" s="5">
+        <v>0</v>
+      </c>
+      <c r="K20" s="11"/>
+      <c r="L20" s="5">
+        <v>1</v>
+      </c>
+      <c r="M20" s="5">
+        <v>2</v>
+      </c>
+      <c r="N20" s="5">
+        <v>1</v>
+      </c>
+      <c r="O20" s="5">
+        <v>0</v>
+      </c>
+      <c r="P20" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="R20" s="5">
+        <v>1</v>
+      </c>
+      <c r="S20" s="5">
+        <v>1</v>
+      </c>
+      <c r="T20" s="5">
+        <v>0</v>
+      </c>
+      <c r="U20" s="5">
+        <v>0</v>
+      </c>
+      <c r="V20" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="5">
-        <v>1</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="5">
+      <c r="A21" s="2">
+        <v>4</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2">
         <v>2</v>
       </c>
-      <c r="D21" s="5">
+      <c r="E21" s="3">
+        <v>1</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1</v>
+      </c>
+      <c r="G21" s="2">
         <v>2</v>
       </c>
-      <c r="E21" s="5">
+      <c r="H21" s="2">
+        <v>1</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0</v>
+      </c>
+      <c r="J21" s="8">
+        <v>0</v>
+      </c>
+      <c r="K21" s="10"/>
+      <c r="L21" s="2">
+        <v>1</v>
+      </c>
+      <c r="M21" s="2">
         <v>2</v>
       </c>
-      <c r="F21" s="5">
+      <c r="N21" s="2">
         <v>2</v>
       </c>
-      <c r="G21" s="5">
+      <c r="O21" s="2">
+        <v>0</v>
+      </c>
+      <c r="P21" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="2">
+        <v>1</v>
+      </c>
+      <c r="S21" s="2">
         <v>2</v>
       </c>
-      <c r="H21" s="5">
-        <v>2</v>
-      </c>
-      <c r="I21" s="5">
-        <v>0</v>
-      </c>
-      <c r="J21" s="5">
-        <v>0</v>
-      </c>
-      <c r="K21" s="11"/>
-      <c r="L21" s="5">
-        <v>2</v>
-      </c>
-      <c r="M21" s="5">
-        <v>4</v>
-      </c>
-      <c r="N21" s="5">
-        <v>2</v>
-      </c>
-      <c r="O21" s="5">
-        <v>0</v>
-      </c>
-      <c r="P21" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="5">
-        <v>2</v>
-      </c>
-      <c r="S21" s="5">
-        <v>2</v>
-      </c>
-      <c r="T21" s="5">
-        <v>4</v>
-      </c>
-      <c r="U21" s="5">
-        <v>0</v>
-      </c>
-      <c r="V21" s="5">
-        <v>2</v>
-      </c>
-      <c r="W21" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="T21" s="2">
+        <v>1</v>
+      </c>
+      <c r="U21" s="2">
+        <v>0</v>
+      </c>
+      <c r="V21" s="2">
+        <v>0</v>
+      </c>
+      <c r="W21" s="8"/>
     </row>
     <row r="22" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="5">
-        <v>2</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="5">
-        <v>1</v>
-      </c>
-      <c r="D22" s="5">
-        <v>2</v>
-      </c>
-      <c r="E22" s="5">
-        <v>1</v>
-      </c>
-      <c r="F22" s="5">
-        <v>1</v>
-      </c>
-      <c r="G22" s="5">
-        <v>2</v>
-      </c>
-      <c r="H22" s="5">
-        <v>1</v>
-      </c>
-      <c r="I22" s="5">
-        <v>0</v>
-      </c>
-      <c r="J22" s="5">
-        <v>0</v>
-      </c>
-      <c r="K22" s="11"/>
-      <c r="L22" s="5">
-        <v>1</v>
-      </c>
-      <c r="M22" s="5">
-        <v>4</v>
-      </c>
-      <c r="N22" s="5">
-        <v>1</v>
-      </c>
-      <c r="O22" s="5">
-        <v>0</v>
-      </c>
-      <c r="P22" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="5">
-        <v>1</v>
-      </c>
-      <c r="S22" s="5">
-        <v>2</v>
-      </c>
-      <c r="T22" s="5">
-        <v>1</v>
-      </c>
-      <c r="U22" s="5">
-        <v>0</v>
-      </c>
-      <c r="V22" s="5">
-        <v>0</v>
-      </c>
+      <c r="A22" s="2">
+        <v>5</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1</v>
+      </c>
+      <c r="G22" s="2">
+        <v>1</v>
+      </c>
+      <c r="H22" s="2">
+        <v>1</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0</v>
+      </c>
+      <c r="J22" s="8">
+        <v>0</v>
+      </c>
+      <c r="K22" s="10"/>
+      <c r="L22" s="2">
+        <v>1</v>
+      </c>
+      <c r="M22" s="2">
+        <v>1</v>
+      </c>
+      <c r="N22" s="2">
+        <v>1</v>
+      </c>
+      <c r="O22" s="2">
+        <v>0</v>
+      </c>
+      <c r="P22" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="2">
+        <v>1</v>
+      </c>
+      <c r="S22" s="2">
+        <v>1</v>
+      </c>
+      <c r="T22" s="2">
+        <v>1</v>
+      </c>
+      <c r="U22" s="2">
+        <v>0</v>
+      </c>
+      <c r="V22" s="2">
+        <v>0</v>
+      </c>
+      <c r="W22" s="8"/>
     </row>
     <row r="23" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="5">
-        <v>3</v>
+      <c r="A23" s="2">
+        <v>6</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C23" s="5">
         <v>1</v>
       </c>
       <c r="D23" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E23" s="5">
         <v>1</v>
@@ -1912,13 +1975,13 @@
         <v>1</v>
       </c>
       <c r="G23" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H23" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" s="5">
         <v>0</v>
@@ -1928,13 +1991,13 @@
         <v>1</v>
       </c>
       <c r="M23" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N23" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P23" s="5">
         <v>0</v>
@@ -1944,7 +2007,7 @@
         <v>1</v>
       </c>
       <c r="S23" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T23" s="5">
         <v>1</v>
@@ -1957,17 +2020,17 @@
       </c>
     </row>
     <row r="24" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="5">
-        <v>4</v>
+      <c r="A24" s="2">
+        <v>7</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C24" s="5">
         <v>1</v>
       </c>
       <c r="D24" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24" s="5">
         <v>1</v>
@@ -1976,13 +2039,13 @@
         <v>1</v>
       </c>
       <c r="G24" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H24" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" s="5">
         <v>0</v>
@@ -1992,13 +2055,13 @@
         <v>1</v>
       </c>
       <c r="M24" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N24" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P24" s="5">
         <v>0</v>
@@ -2008,7 +2071,7 @@
         <v>1</v>
       </c>
       <c r="S24" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T24" s="5">
         <v>1</v>
@@ -2021,11 +2084,11 @@
       </c>
     </row>
     <row r="25" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="5">
-        <v>5</v>
+      <c r="A25" s="2">
+        <v>8</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C25" s="5">
         <v>1</v>
@@ -2034,7 +2097,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="5">
         <v>1</v>
@@ -2049,7 +2112,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25" s="11"/>
       <c r="L25" s="5">
@@ -2065,7 +2128,7 @@
         <v>0</v>
       </c>
       <c r="P25" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q25" s="11"/>
       <c r="R25" s="5">
@@ -2081,85 +2144,411 @@
         <v>0</v>
       </c>
       <c r="V25" s="5">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="15"/>
+      <c r="S26" s="15"/>
+      <c r="T26" s="15"/>
+      <c r="U26" s="15"/>
+      <c r="V26" s="15"/>
+      <c r="W26" s="15"/>
     </row>
     <row r="27" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="5"/>
+      <c r="A27" s="5">
+        <v>1</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="5">
+        <v>2</v>
+      </c>
+      <c r="D27" s="5">
+        <v>2</v>
+      </c>
+      <c r="E27" s="5">
+        <v>2</v>
+      </c>
+      <c r="F27" s="5">
+        <v>2</v>
+      </c>
+      <c r="G27" s="5">
+        <v>2</v>
+      </c>
+      <c r="H27" s="5">
+        <v>2</v>
+      </c>
+      <c r="I27" s="5">
+        <v>0</v>
+      </c>
+      <c r="J27" s="5">
+        <v>0</v>
+      </c>
+      <c r="K27" s="11"/>
+      <c r="L27" s="5">
+        <v>2</v>
+      </c>
+      <c r="M27" s="5">
+        <v>4</v>
+      </c>
+      <c r="N27" s="5">
+        <v>2</v>
+      </c>
+      <c r="O27" s="5">
+        <v>0</v>
+      </c>
+      <c r="P27" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="5">
+        <v>2</v>
+      </c>
+      <c r="S27" s="5">
+        <v>2</v>
+      </c>
+      <c r="T27" s="5">
+        <v>4</v>
+      </c>
+      <c r="U27" s="5">
+        <v>0</v>
+      </c>
+      <c r="V27" s="5">
+        <v>2</v>
+      </c>
+      <c r="W27" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
+        <v>2</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="5">
+        <v>1</v>
+      </c>
+      <c r="D28" s="5">
+        <v>2</v>
+      </c>
+      <c r="E28" s="5">
+        <v>1</v>
+      </c>
+      <c r="F28" s="5">
+        <v>1</v>
+      </c>
+      <c r="G28" s="5">
+        <v>2</v>
+      </c>
+      <c r="H28" s="5">
+        <v>1</v>
+      </c>
+      <c r="I28" s="5">
+        <v>0</v>
+      </c>
+      <c r="J28" s="5">
+        <v>0</v>
+      </c>
+      <c r="K28" s="11"/>
+      <c r="L28" s="5">
+        <v>1</v>
+      </c>
+      <c r="M28" s="5">
+        <v>4</v>
+      </c>
+      <c r="N28" s="5">
+        <v>1</v>
+      </c>
+      <c r="O28" s="5">
+        <v>0</v>
+      </c>
+      <c r="P28" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="5">
+        <v>1</v>
+      </c>
+      <c r="S28" s="5">
+        <v>2</v>
+      </c>
+      <c r="T28" s="5">
+        <v>1</v>
+      </c>
+      <c r="U28" s="5">
+        <v>0</v>
+      </c>
+      <c r="V28" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="5"/>
+      <c r="A29" s="5">
+        <v>3</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="5">
+        <v>1</v>
+      </c>
+      <c r="D29" s="5">
+        <v>2</v>
+      </c>
+      <c r="E29" s="5">
+        <v>1</v>
+      </c>
+      <c r="F29" s="5">
+        <v>1</v>
+      </c>
+      <c r="G29" s="5">
+        <v>2</v>
+      </c>
+      <c r="H29" s="5">
+        <v>1</v>
+      </c>
+      <c r="I29" s="5">
+        <v>0</v>
+      </c>
+      <c r="J29" s="5">
+        <v>0</v>
+      </c>
+      <c r="K29" s="11"/>
+      <c r="L29" s="5">
+        <v>1</v>
+      </c>
+      <c r="M29" s="5">
+        <v>4</v>
+      </c>
+      <c r="N29" s="5">
+        <v>1</v>
+      </c>
+      <c r="O29" s="5">
+        <v>0</v>
+      </c>
+      <c r="P29" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="5">
+        <v>1</v>
+      </c>
+      <c r="S29" s="5">
+        <v>2</v>
+      </c>
+      <c r="T29" s="5">
+        <v>1</v>
+      </c>
+      <c r="U29" s="5">
+        <v>0</v>
+      </c>
+      <c r="V29" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="5"/>
+      <c r="A30" s="5">
+        <v>4</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="5">
+        <v>1</v>
+      </c>
+      <c r="D30" s="5">
+        <v>2</v>
+      </c>
+      <c r="E30" s="5">
+        <v>1</v>
+      </c>
+      <c r="F30" s="5">
+        <v>1</v>
+      </c>
+      <c r="G30" s="5">
+        <v>2</v>
+      </c>
+      <c r="H30" s="5">
+        <v>1</v>
+      </c>
+      <c r="I30" s="5">
+        <v>0</v>
+      </c>
+      <c r="J30" s="5">
+        <v>0</v>
+      </c>
+      <c r="K30" s="11"/>
+      <c r="L30" s="5">
+        <v>1</v>
+      </c>
+      <c r="M30" s="5">
+        <v>4</v>
+      </c>
+      <c r="N30" s="5">
+        <v>1</v>
+      </c>
+      <c r="O30" s="5">
+        <v>0</v>
+      </c>
+      <c r="P30" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="5">
+        <v>1</v>
+      </c>
+      <c r="S30" s="5">
+        <v>2</v>
+      </c>
+      <c r="T30" s="5">
+        <v>1</v>
+      </c>
+      <c r="U30" s="5">
+        <v>0</v>
+      </c>
+      <c r="V30" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="5"/>
-    </row>
-    <row r="32" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="5"/>
-    </row>
-    <row r="33" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K33" s="11"/>
-      <c r="Q33" s="11"/>
-    </row>
-    <row r="34" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K34" s="11"/>
-      <c r="Q34" s="11"/>
-    </row>
-    <row r="35" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K35" s="11"/>
-      <c r="Q35" s="11"/>
-    </row>
-    <row r="36" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K36" s="11"/>
-      <c r="Q36" s="11"/>
-    </row>
-    <row r="37" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K37" s="11"/>
-      <c r="Q37" s="11"/>
-    </row>
-    <row r="38" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K38" s="11"/>
-      <c r="Q38" s="11"/>
-    </row>
-    <row r="39" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
+        <v>5</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="5">
+        <v>1</v>
+      </c>
+      <c r="D31" s="5">
+        <v>1</v>
+      </c>
+      <c r="E31" s="5">
+        <v>0</v>
+      </c>
+      <c r="F31" s="5">
+        <v>1</v>
+      </c>
+      <c r="G31" s="5">
+        <v>1</v>
+      </c>
+      <c r="H31" s="5">
+        <v>1</v>
+      </c>
+      <c r="I31" s="5">
+        <v>0</v>
+      </c>
+      <c r="J31" s="5">
+        <v>1</v>
+      </c>
+      <c r="K31" s="11"/>
+      <c r="L31" s="5">
+        <v>1</v>
+      </c>
+      <c r="M31" s="5">
+        <v>2</v>
+      </c>
+      <c r="N31" s="5">
+        <v>1</v>
+      </c>
+      <c r="O31" s="5">
+        <v>0</v>
+      </c>
+      <c r="P31" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="5">
+        <v>1</v>
+      </c>
+      <c r="S31" s="5">
+        <v>1</v>
+      </c>
+      <c r="T31" s="5">
+        <v>1</v>
+      </c>
+      <c r="U31" s="5">
+        <v>0</v>
+      </c>
+      <c r="V31" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="5"/>
+    </row>
+    <row r="35" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="5"/>
+    </row>
+    <row r="36" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="5"/>
+    </row>
+    <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="5"/>
+    </row>
+    <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="5"/>
+    </row>
+    <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K39" s="11"/>
       <c r="Q39" s="11"/>
     </row>
-    <row r="40" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K40" s="11"/>
       <c r="Q40" s="11"/>
     </row>
-    <row r="41" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K41" s="11"/>
       <c r="Q41" s="11"/>
     </row>
-    <row r="42" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K42" s="11"/>
       <c r="Q42" s="11"/>
     </row>
-    <row r="43" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K43" s="11"/>
       <c r="Q43" s="11"/>
     </row>
-    <row r="44" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K44" s="11"/>
       <c r="Q44" s="11"/>
     </row>
-    <row r="45" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K45" s="11"/>
       <c r="Q45" s="11"/>
     </row>
-    <row r="46" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K46" s="11"/>
       <c r="Q46" s="11"/>
     </row>
-    <row r="47" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K47" s="11"/>
       <c r="Q47" s="11"/>
     </row>
-    <row r="48" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K48" s="11"/>
       <c r="Q48" s="11"/>
     </row>
@@ -2235,27 +2624,27 @@
       <c r="K66" s="11"/>
       <c r="Q66" s="11"/>
     </row>
-    <row r="67" spans="11:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K67" s="11"/>
       <c r="Q67" s="11"/>
     </row>
-    <row r="68" spans="11:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="68" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K68" s="11"/>
       <c r="Q68" s="11"/>
     </row>
-    <row r="69" spans="11:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="69" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K69" s="11"/>
       <c r="Q69" s="11"/>
     </row>
-    <row r="70" spans="11:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K70" s="11"/>
       <c r="Q70" s="11"/>
     </row>
-    <row r="71" spans="11:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="71" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K71" s="11"/>
       <c r="Q71" s="11"/>
     </row>
-    <row r="72" spans="11:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K72" s="11"/>
       <c r="Q72" s="11"/>
     </row>
@@ -6015,11 +6404,35 @@
       <c r="K1011" s="11"/>
       <c r="Q1011" s="11"/>
     </row>
+    <row r="1012" spans="11:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K1012" s="11"/>
+      <c r="Q1012" s="11"/>
+    </row>
+    <row r="1013" spans="11:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K1013" s="11"/>
+      <c r="Q1013" s="11"/>
+    </row>
+    <row r="1014" spans="11:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K1014" s="11"/>
+      <c r="Q1014" s="11"/>
+    </row>
+    <row r="1015" spans="11:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K1015" s="11"/>
+      <c r="Q1015" s="11"/>
+    </row>
+    <row r="1016" spans="11:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K1016" s="11"/>
+      <c r="Q1016" s="11"/>
+    </row>
+    <row r="1017" spans="11:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K1017" s="11"/>
+      <c r="Q1017" s="11"/>
+    </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A20:W20"/>
+    <mergeCell ref="A26:W26"/>
     <mergeCell ref="A3:W3"/>
-    <mergeCell ref="A10:W10"/>
+    <mergeCell ref="A17:W17"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="F1:K1"/>
     <mergeCell ref="L1:Q1"/>

</xml_diff>